<commit_message>
Correciones menores en varios archivos
</commit_message>
<xml_diff>
--- a/Files/productos.xlsx
+++ b/Files/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cursos y Practica\Informatorio\Dataset_Laboratorio\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404666E2-EB20-484A-8AE7-38EE78766F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6430FC63-1B91-43B0-8E5B-826D7D0830A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{065C86F8-B644-48F6-92B5-A0C557740D14}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Cafetera Nespresso</t>
-  </si>
-  <si>
-    <t>129.95</t>
   </si>
   <si>
     <t>Cámara Canon EOS</t>
@@ -682,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1E6356-79F7-4C0A-9FE5-BFA6E623C900}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,18 +1113,12 @@
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>25.99</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F19" s="4"/>
       <c r="G19" s="2">
         <v>45129</v>
       </c>
@@ -1137,13 +1128,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1">
         <v>119.8</v>
@@ -1160,13 +1151,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1">
         <v>15.9</v>
@@ -1183,19 +1174,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="1">
         <v>59.8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="2">
         <v>45163</v>
@@ -1206,19 +1197,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1">
         <v>3.9980000000000002</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="2">
         <v>44967</v>
@@ -1229,19 +1220,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1">
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="1">
         <v>13.99</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G24" s="2">
         <v>45000</v>
@@ -1252,19 +1243,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1">
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1">
         <v>29.8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="2">
         <v>44956</v>
@@ -1275,19 +1266,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1">
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1">
         <v>7.9980000000000002</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="2">
         <v>45051</v>
@@ -1298,13 +1289,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1">
         <v>31.8</v>
@@ -1321,13 +1312,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
         <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1">
         <v>17.989999999999998</v>
@@ -1344,19 +1335,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1">
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="1">
         <v>7.1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="2">
         <v>45026</v>
@@ -1367,19 +1358,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1">
         <v>50</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="1">
         <v>2.5979999999999999</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="2">
         <v>45146</v>
@@ -1391,19 +1382,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1">
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="1">
         <v>11.997999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" s="2">
         <v>45010</v>
@@ -1414,19 +1405,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1">
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="1">
         <v>15.8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G32" s="2">
         <v>45076</v>
@@ -1437,19 +1428,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="1">
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1">
         <v>4.99</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" s="2">
         <v>45122</v>
@@ -1460,19 +1451,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1">
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="1">
         <v>9</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G34" s="2">
         <v>44977</v>
@@ -1483,19 +1474,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="1">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="1">
         <v>7.9980000000000002</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G35" s="2">
         <v>45170</v>
@@ -1506,19 +1497,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1">
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E36" s="1">
         <v>5.9</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36" s="2">
         <v>44936</v>
@@ -1529,19 +1520,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1">
         <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="1">
         <v>5.9</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G37" s="2">
         <v>44936</v>
@@ -1552,7 +1543,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
@@ -1560,7 +1551,7 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" s="2">
         <v>45170</v>

</xml_diff>

<commit_message>
Cambios en el archivo excel
</commit_message>
<xml_diff>
--- a/Files/productos.xlsx
+++ b/Files/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cursos y Practica\Informatorio\Dataset_Laboratorio\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6430FC63-1B91-43B0-8E5B-826D7D0830A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33C13B5-7488-4D3F-83E2-D9CF245D13D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{065C86F8-B644-48F6-92B5-A0C557740D14}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{065C86F8-B644-48F6-92B5-A0C557740D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -42,21 +42,9 @@
     <t>nombre_prod</t>
   </si>
   <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Precio en Dolares</t>
-  </si>
-  <si>
-    <t>Precio en pesos</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>Fecha_Ingreso</t>
-  </si>
-  <si>
     <t>Laptop HP EliteBook</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t>iPhone 13</t>
   </si>
   <si>
-    <t>699.00</t>
-  </si>
-  <si>
     <t>Samsung Galaxy S22</t>
   </si>
   <si>
@@ -81,9 +66,6 @@
     <t>Smart TV LG 4K</t>
   </si>
   <si>
-    <t>549.50</t>
-  </si>
-  <si>
     <t>Refrigerador Whirlpool</t>
   </si>
   <si>
@@ -204,9 +186,6 @@
     <t>Raqueta de tenis</t>
   </si>
   <si>
-    <t>69.95</t>
-  </si>
-  <si>
     <t>Set de maletas</t>
   </si>
   <si>
@@ -289,6 +268,21 @@
   </si>
   <si>
     <t>29.50</t>
+  </si>
+  <si>
+    <t>Stock_num</t>
+  </si>
+  <si>
+    <t>PrecioEnDolares_num</t>
+  </si>
+  <si>
+    <t>Fecha_Ingreso_date</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>PrecioEnpesos_num</t>
   </si>
 </sst>
 </file>
@@ -677,22 +671,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1E6356-79F7-4C0A-9FE5-BFA6E623C900}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,361 +694,362 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <v>179.99799999999999</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
         <v>45056</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
+      <c r="D3" s="1">
+        <v>699</v>
       </c>
       <c r="E3" s="1">
         <v>139.80000000000001</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>45092</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>149.99799999999999</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
         <v>45036</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E5" s="1">
         <v>109.9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2">
         <v>45108</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1">
         <v>159.80000000000001</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="2">
-        <v>44997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2">
         <v>44985</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2">
         <v>45143</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1">
         <v>9.1980000000000004</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2">
         <v>45179</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>17.998000000000001</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G10" s="2">
         <v>44941</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
         <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>25.9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G11" s="2">
         <v>45068</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1">
         <v>79.8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G12" s="2">
         <v>45107</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1">
         <v>31.95</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2">
         <v>45125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1">
         <v>15.997999999999999</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2">
         <v>45021</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="33" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1">
         <v>5.9980000000000002</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2">
         <v>44993</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1">
         <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1">
         <v>9.98</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2">
         <v>45150</v>
@@ -1065,19 +1060,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1">
         <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1">
         <v>17.8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G17" s="2">
         <v>45174</v>
@@ -1088,19 +1083,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1">
         <v>39.997999999999998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G18" s="2">
         <v>45060</v>
@@ -1111,7 +1106,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1128,19 +1123,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1">
         <v>119.8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G20" s="2">
         <v>45087</v>
@@ -1151,19 +1146,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1">
         <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1">
         <v>15.9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G21" s="2">
         <v>45034</v>
@@ -1174,19 +1169,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E22" s="1">
         <v>59.8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G22" s="2">
         <v>45163</v>
@@ -1197,19 +1192,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1">
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
         <v>3.9980000000000002</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G23" s="2">
         <v>44967</v>
@@ -1220,19 +1215,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1">
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E24" s="1">
         <v>13.99</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G24" s="2">
         <v>45000</v>
@@ -1243,19 +1238,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1">
         <v>8</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>58</v>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E25" s="1">
         <v>29.8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G25" s="2">
         <v>44956</v>
@@ -1266,19 +1261,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1">
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1">
         <v>7.9980000000000002</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G26" s="2">
         <v>45051</v>
@@ -1289,19 +1284,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1">
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E27" s="1">
         <v>31.8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G27" s="2">
         <v>45119</v>
@@ -1312,19 +1307,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1">
         <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E28" s="1">
         <v>17.989999999999998</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G28" s="2">
         <v>45097</v>
@@ -1335,19 +1330,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1">
         <v>7.1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G29" s="2">
         <v>45026</v>
@@ -1358,19 +1353,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1">
         <v>50</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E30" s="1">
         <v>2.5979999999999999</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G30" s="2">
         <v>45146</v>
@@ -1382,19 +1377,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1">
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E31" s="1">
         <v>11.997999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G31" s="2">
         <v>45010</v>
@@ -1405,19 +1400,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1">
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E32" s="1">
         <v>15.8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G32" s="2">
         <v>45076</v>
@@ -1428,19 +1423,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1">
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E33" s="1">
         <v>4.99</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G33" s="2">
         <v>45122</v>
@@ -1451,19 +1446,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1">
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1">
         <v>9</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G34" s="2">
         <v>44977</v>
@@ -1474,19 +1469,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E35" s="1">
         <v>7.9980000000000002</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G35" s="2">
         <v>45170</v>
@@ -1497,19 +1492,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1">
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E36" s="1">
         <v>5.9</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G36" s="2">
         <v>44936</v>
@@ -1520,19 +1515,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1">
         <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E37" s="1">
         <v>5.9</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G37" s="2">
         <v>44936</v>
@@ -1543,7 +1538,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
@@ -1551,7 +1546,7 @@
         <v>7.9980000000000002</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G38" s="2">
         <v>45170</v>

</xml_diff>